<commit_message>
add interpolation discriminator with generic approach and Perterson Coefficient method, add operations matrix handler, optimize & refactoring code for better understanding and performances
</commit_message>
<xml_diff>
--- a/dataset/models/input/Common Formulas+Constants.xlsx
+++ b/dataset/models/input/Common Formulas+Constants.xlsx
@@ -457,7 +457,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,6 +467,12 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -526,10 +532,10 @@
     <xf xfId="0" numFmtId="165" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -547,7 +553,7 @@
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
@@ -887,7 +893,7 @@
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
       <c r="A2" s="4"/>
       <c r="B2" s="2" t="s">
         <v>32</v>
@@ -902,7 +908,7 @@
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
       <c r="A3" s="4"/>
       <c r="B3" s="2" t="s">
         <v>35</v>
@@ -937,7 +943,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
       <c r="A6" s="4"/>
       <c r="B6" s="2" t="s">
         <v>39</v>
@@ -952,7 +958,7 @@
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
       <c r="A7" s="4"/>
       <c r="B7" s="14"/>
       <c r="C7" s="15"/>
@@ -1032,7 +1038,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>54</v>
@@ -1047,7 +1053,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="4"/>
       <c r="B14" s="2"/>
       <c r="C14" s="15"/>
@@ -1155,7 +1161,7 @@
       <c r="F21" s="4"/>
       <c r="G21" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
       <c r="A22" s="4"/>
       <c r="B22" s="2" t="s">
         <v>48</v>
@@ -1170,7 +1176,7 @@
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
       <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
         <v>65</v>
@@ -1185,7 +1191,7 @@
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
       <c r="A24" s="4"/>
       <c r="B24" s="2" t="s">
         <v>68</v>
@@ -1200,7 +1206,7 @@
       <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
       <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>71</v>
@@ -1215,7 +1221,7 @@
       <c r="F25" s="4"/>
       <c r="G25" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
       <c r="A26" s="4"/>
       <c r="B26" s="2" t="s">
         <v>51</v>
@@ -1230,7 +1236,7 @@
       <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
       <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>75</v>
@@ -1245,7 +1251,7 @@
       <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
       <c r="A28" s="4"/>
       <c r="B28" s="2" t="s">
         <v>77</v>
@@ -1260,7 +1266,7 @@
       <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
       <c r="A29" s="1"/>
       <c r="B29" s="2" t="s">
         <v>54</v>

</xml_diff>